<commit_message>
traitement de donnees de vente de produits pharmaceutique
</commit_message>
<xml_diff>
--- a/exercice4.1/test_vente.xlsx
+++ b/exercice4.1/test_vente.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bili_\Documents\workspace\python-tutorials\exercice4.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4155D08F-D454-415E-BE75-A88EF68C4B7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B820AC62-DAC4-4081-A245-32B4395FED24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$E$16</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +450,7 @@
     <col min="1" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -480,8 +483,12 @@
       <c r="E2" s="1">
         <v>1.95</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>+E2*D2</f>
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -497,8 +504,12 @@
       <c r="E3" s="1">
         <v>2.1800000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F16" si="0">+E3*D3</f>
+        <v>87.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -514,8 +525,12 @@
       <c r="E4" s="1">
         <v>2.1800000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>152.60000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -531,8 +546,12 @@
       <c r="E5" s="1">
         <v>2.76</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>33.119999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -548,8 +567,12 @@
       <c r="E6" s="1">
         <v>3.39</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>152.55000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -565,8 +588,12 @@
       <c r="E7" s="1">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>133.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -582,8 +609,12 @@
       <c r="E8" s="1">
         <v>2.14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -599,8 +630,12 @@
       <c r="E9" s="1">
         <v>10.67</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>426.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -616,8 +651,12 @@
       <c r="E10" s="1">
         <v>15.77</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1103.8999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -633,8 +672,12 @@
       <c r="E11" s="1">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -650,8 +693,12 @@
       <c r="E12" s="1">
         <v>1.88</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -667,8 +714,12 @@
       <c r="E13" s="1">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -684,8 +735,12 @@
       <c r="E14" s="1">
         <v>3.04</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>182.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -701,8 +756,12 @@
       <c r="E15" s="1">
         <v>1.94</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>58.199999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -718,8 +777,19 @@
       <c r="E16" s="1">
         <v>2.5499999999999998</v>
       </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f>SUM(F2:F16)</f>
+        <v>3312.72</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E16" xr:uid="{75CBC895-D972-45BE-B57C-D45C9AB1801B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>